<commit_message>
Fix URL File Test
</commit_message>
<xml_diff>
--- a/test-resources/data/RESULT_TEST_LOGIN.xlsx
+++ b/test-resources/data/RESULT_TEST_LOGIN.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="50">
   <si>
     <t>STT</t>
   </si>
@@ -47,46 +47,58 @@
     <t>1</t>
   </si>
   <si>
+    <t>taikhoanchuatontai</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Test Login</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:58:33 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>cus01</t>
+  </si>
+  <si>
+    <t>MatKhau123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:58:36 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>cust01</t>
   </si>
   <si>
     <t>MatKhau@123</t>
   </si>
   <si>
-    <t>Test Login</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:14:11 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>D:/xxx/xxx/DU_AN_TOT_NGHIEP/Code/GodEShop/test-resources/images/failure-1656666859799.png</t>
-  </si>
-  <si>
-    <t>Full Image</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t xml:space="preserve">07:58:39 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>MatKhau</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:14:24 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>3</t>
+    <t xml:space="preserve">07:58:43 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>cust02</t>
@@ -95,10 +107,10 @@
     <t>124</t>
   </si>
   <si>
-    <t xml:space="preserve">16:14:27 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>4</t>
+    <t xml:space="preserve">07:58:46 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>cus12345</t>
@@ -107,10 +119,10 @@
     <t>12345</t>
   </si>
   <si>
-    <t xml:space="preserve">16:14:30 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>5</t>
+    <t xml:space="preserve">07:58:48 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
   <si>
     <t>cust1102</t>
@@ -119,46 +131,37 @@
     <t>123</t>
   </si>
   <si>
-    <t xml:space="preserve">16:14:33 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:14:36 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:14:39 | 01-07-2022 </t>
+    <t xml:space="preserve">07:58:51 | 20-07-2022 </t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
+    <t xml:space="preserve">07:58:54 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07:58:56 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>user02</t>
   </si>
   <si>
-    <t xml:space="preserve">16:14:42 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>9</t>
+    <t xml:space="preserve">07:58:59 | 20-07-2022 </t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>pppp</t>
   </si>
   <si>
-    <t xml:space="preserve">16:14:45 | 01-07-2022 </t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>taikhoanchuatontai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:14:49 | 01-07-2022 </t>
+    <t xml:space="preserve">07:59:01 | 20-07-2022 </t>
   </si>
 </sst>
 </file>
@@ -195,8 +198,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
@@ -237,66 +243,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1819275" cy="1009650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="10" max="10" width="27.34375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="18.50390625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="14.53125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.08203125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="9.234375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="8.37890625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="7.2265625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.59375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.67578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.20703125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="5.078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true">
@@ -331,7 +294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="80.0" customHeight="true">
+    <row r="2" s="3" customFormat="true">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -345,7 +308,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -357,76 +320,76 @@
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" s="4" customFormat="true">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" s="5" customFormat="true">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" s="6" customFormat="true">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -438,24 +401,24 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" s="7" customFormat="true">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -467,24 +430,24 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" s="8" customFormat="true">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -496,25 +459,25 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" s="9" customFormat="true">
       <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
@@ -525,13 +488,13 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" s="10" customFormat="true">
@@ -539,93 +502,118 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
       <c r="I9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" s="11" customFormat="true">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" t="s">
-        <v>45</v>
-      </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" s="12" customFormat="true">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
         <v>46</v>
       </c>
-      <c r="B11" t="s">
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" s="13" customFormat="true">
+      <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="I11" t="s">
-        <v>23</v>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId11"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>